<commit_message>
treemap w/ only agrifood emissions commit
</commit_message>
<xml_diff>
--- a/Ch3_Roe2021/output/roe2021.xlsx
+++ b/Ch3_Roe2021/output/roe2021.xlsx
@@ -17133,6 +17133,13 @@
       <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     </lcf76f155ced4ddcb4097134ff3c332f>
     <TaxCatchAll xmlns="651cb2ee-101c-46d8-8d18-354772623485" xsi:nil="true"/>
+    <SharedWithUsers xmlns="651cb2ee-101c-46d8-8d18-354772623485">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
   </documentManagement>
 </p:properties>
 </file>

</xml_diff>